<commit_message>
Added data type to dictionary: ID, traffic_data, safety_measures, location_data, geometry_data.
</commit_message>
<xml_diff>
--- a/references/Dictionnaire_final.xlsx
+++ b/references/Dictionnaire_final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jordan/Documents/School/University/Master's degree/Winter 2024/MATH 60611A - Advanced Statistical Learning/RoadSafety_ASL.H2024/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jordan/Documents/School/University/Master's degree/Winter 2024/MATH 60611A - Advanced Statistical Learning/roadsafety_project/references/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E7756A-D3E4-6445-9489-CF66BCEC37AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367F8888-9AC4-024F-9397-53FF67885747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{FC27DABD-5B5C-0443-85BA-617F49EB5D14}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{FC27DABD-5B5C-0443-85BA-617F49EB5D14}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="126">
   <si>
     <t>int_no</t>
   </si>
@@ -396,6 +396,24 @@
   </si>
   <si>
     <t xml:space="preserve"> presence of a restricted or protected  left turn lane at the intersection</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>traffic_data</t>
+  </si>
+  <si>
+    <t>geometry_data</t>
+  </si>
+  <si>
+    <t>safety_measures</t>
+  </si>
+  <si>
+    <t>location_data</t>
   </si>
 </sst>
 </file>
@@ -775,9 +793,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43D0810-E943-7A4C-B93A-00C33991F0EE}">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
@@ -785,486 +803,667 @@
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="68.83203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C58" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C59" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>113</v>
+      </c>
+      <c r="C60" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned up dataset and added code to import data dict.
</commit_message>
<xml_diff>
--- a/references/Dictionnaire_final.xlsx
+++ b/references/Dictionnaire_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jordan/Documents/School/University/Master's degree/Winter 2024/MATH 60611A - Advanced Statistical Learning/roadsafety_project/references/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367F8888-9AC4-024F-9397-53FF67885747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2620BD1D-81BD-6042-8FF8-04C74E7CA0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{FC27DABD-5B5C-0443-85BA-617F49EB5D14}"/>
   </bookViews>
@@ -113,21 +113,12 @@
     <t>fti</t>
   </si>
   <si>
-    <t>cli </t>
-  </si>
-  <si>
     <t xml:space="preserve"> number of pedestrian-vehicle left turning potential interactions over each 15 min intervals during the observed counting period</t>
   </si>
   <si>
-    <t>cri </t>
-  </si>
-  <si>
     <t xml:space="preserve"> number of pedestrian-vehicle right turning potential interactions over each 15 min intervals during the observed counting period </t>
   </si>
   <si>
-    <t>cti </t>
-  </si>
-  <si>
     <t xml:space="preserve"> number of pedestrian-vehicle prohibited interactions over each 15 min intervals during the observed counting period </t>
   </si>
   <si>
@@ -143,9 +134,6 @@
     <t xml:space="preserve"> log of pi (if pi=0 then ln_pi=0)</t>
   </si>
   <si>
-    <t>ln_fi </t>
-  </si>
-  <si>
     <t xml:space="preserve"> log of fi</t>
   </si>
   <si>
@@ -414,6 +402,18 @@
   </si>
   <si>
     <t>location_data</t>
+  </si>
+  <si>
+    <t>cli</t>
+  </si>
+  <si>
+    <t>cri</t>
+  </si>
+  <si>
+    <t>cti</t>
+  </si>
+  <si>
+    <t>ln_fi</t>
   </si>
 </sst>
 </file>
@@ -795,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43D0810-E943-7A4C-B93A-00C33991F0EE}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -808,13 +808,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -825,7 +825,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -836,7 +836,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -847,7 +847,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -858,7 +858,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -869,7 +869,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -880,7 +880,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -891,7 +891,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -902,7 +902,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -913,7 +913,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -924,7 +924,7 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -935,7 +935,7 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -943,10 +943,10 @@
         <v>22</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -954,10 +954,10 @@
         <v>23</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -965,505 +965,505 @@
         <v>24</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="C16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>27</v>
+        <v>123</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>35</v>
+        <v>125</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C33" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C34" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C35" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C37" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C38" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C39" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C40" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C41" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C42" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C43" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C44" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C45" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C46" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C47" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C48" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C49" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C50" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C51" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C52" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C53" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C54" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C55" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C56" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C57" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C58" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C59" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C60" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added poisson reg test and finalized boosting model with transformation.
</commit_message>
<xml_diff>
--- a/references/Dictionnaire_final.xlsx
+++ b/references/Dictionnaire_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jordan/Documents/School/University/Master's degree/Winter 2024/MATH 60611A - Advanced Statistical Learning/roadsafety_project/references/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2620BD1D-81BD-6042-8FF8-04C74E7CA0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F2C7C5-A45E-ED46-9A21-13F42E60AB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{FC27DABD-5B5C-0443-85BA-617F49EB5D14}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="127">
   <si>
     <t>int_no</t>
   </si>
@@ -414,6 +414,9 @@
   </si>
   <si>
     <t>ln_fi</t>
+  </si>
+  <si>
+    <t>predictor</t>
   </si>
 </sst>
 </file>
@@ -795,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43D0810-E943-7A4C-B93A-00C33991F0EE}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1012,7 +1015,7 @@
         <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>